<commit_message>
Separating source code with multiples .py files
</commit_message>
<xml_diff>
--- a/Data/bills_of_materials.xlsx
+++ b/Data/bills_of_materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://globalimi-my.sharepoint.com/personal/bryndell_torio_global-imi_com/Documents/Design/Training/pyxl_training/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://globalimi-my.sharepoint.com/personal/bryndell_torio_global-imi_com/Documents/Design/Training/bomgen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{5DC35224-952F-4A00-9BB3-595198C15376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F40BBADB-8A60-4378-85F2-5A2120929FCF}"/>
@@ -2567,7 +2567,7 @@
   <dimension ref="A1:L168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" activeCellId="1" sqref="A1:A2 A1:XFD1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>